<commit_message>
ajout des alt sur toutes les images et du changement de résolution pour les slider en 1902x880/1903x887 et 440xX ou Yx440
</commit_message>
<xml_diff>
--- a/Liste des optimisations .xlsx
+++ b/Liste des optimisations .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allan\Documents\OpenClassrooms\Nina-Carducci-Dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DCA87C-0C32-4DCF-8B23-4EDB9E4F6A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6C827A-2395-4FD5-AFEB-5915E82F3E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2625" windowWidth="21600" windowHeight="11295" xr2:uid="{21137332-F5F5-4B18-AB0F-0525C6982461}"/>
+    <workbookView xWindow="-19950" yWindow="0" windowWidth="20055" windowHeight="15585" xr2:uid="{21137332-F5F5-4B18-AB0F-0525C6982461}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>performance</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Modification état</t>
+  </si>
+  <si>
+    <t>à faire</t>
   </si>
 </sst>
 </file>
@@ -190,8 +193,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1D57D991-DA3D-44B8-8419-B6A5A77139E6}" name="Tableau8" displayName="Tableau8" ref="A20:B26" totalsRowShown="0">
-  <autoFilter ref="A20:B26" xr:uid="{1D57D991-DA3D-44B8-8419-B6A5A77139E6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1D57D991-DA3D-44B8-8419-B6A5A77139E6}" name="Tableau8" displayName="Tableau8" ref="A20:B28" totalsRowShown="0">
+  <autoFilter ref="A20:B28" xr:uid="{1D57D991-DA3D-44B8-8419-B6A5A77139E6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{15B79476-2AE9-49C7-9AAD-AF3937CC9523}" name="Modification état"/>
     <tableColumn id="2" xr3:uid="{4F9DA640-E57C-415B-A086-0B7108E2A25E}" name="Accessibilité" dataDxfId="1"/>
@@ -579,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FA33F3-59C9-40C8-A3C4-A888687FE5A6}">
   <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,66 +603,105 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
@@ -673,33 +715,61 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
       <c r="B23" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
       <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
       <c r="B25" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
       <c r="B26" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -711,16 +781,25 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
       <c r="B31" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
       <c r="B32" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
       <c r="B33" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>